<commit_message>
Add io column rename + rename column names
</commit_message>
<xml_diff>
--- a/tno/quantum/problems/portfolio_optimization/datasets/rabodata.xlsx
+++ b/tno/quantum/problems/portfolio_optimization/datasets/rabodata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lindesgvd\Desktop\Projects\portfolio-optimization\tno\quantum\problems\portfolio_optimization\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wezemanrs\Desktop\projects\Quantum-projects\QuantumToolbox\PROBLEMS\portfolio-optimization\tno\quantum\problems\portfolio_optimization\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43912144-29C9-4B2B-A7ED-A3111D6E5B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F09AAD-0A9B-44EB-8BCE-AB295289DC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="360" windowWidth="20955" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,25 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
-  <si>
-    <t>out_2021</t>
-  </si>
-  <si>
-    <t>out_2030_min</t>
-  </si>
-  <si>
-    <t>out_2030_max</t>
-  </si>
-  <si>
-    <t>income_2021</t>
-  </si>
-  <si>
-    <t>regcap_2021</t>
-  </si>
-  <si>
-    <t>emis_intens_2021</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>AP - Processing COUNTRY 1</t>
   </si>
@@ -209,7 +191,28 @@
     <t>Packaging &amp; Logistics COUNTRY 4</t>
   </si>
   <si>
-    <t>emis_intens_2030</t>
+    <t>out_now</t>
+  </si>
+  <si>
+    <t>out_future_min</t>
+  </si>
+  <si>
+    <t>out_future_max</t>
+  </si>
+  <si>
+    <t>emis_intens_now</t>
+  </si>
+  <si>
+    <t>emis_intens_future</t>
+  </si>
+  <si>
+    <t>income_now</t>
+  </si>
+  <si>
+    <t>regcap_now</t>
+  </si>
+  <si>
+    <t>asset</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -254,7 +257,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,15 +546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
@@ -560,31 +565,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>10.199999999999999</v>
@@ -615,7 +623,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>600</v>
@@ -646,7 +654,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
@@ -677,7 +685,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>800</v>
@@ -708,7 +716,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>40</v>
@@ -738,7 +746,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>200</v>
@@ -768,7 +776,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
@@ -798,7 +806,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>500</v>
@@ -828,7 +836,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>9.9</v>
@@ -858,7 +866,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>1250</v>
@@ -888,7 +896,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>70</v>
@@ -918,7 +926,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>700</v>
@@ -948,7 +956,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -978,7 +986,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>30</v>
@@ -1008,7 +1016,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>1200</v>
@@ -1038,7 +1046,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>10</v>
@@ -1068,7 +1076,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>800</v>
@@ -1098,7 +1106,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>9.6</v>
@@ -1128,7 +1136,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>1000</v>
@@ -1158,7 +1166,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>50</v>
@@ -1188,7 +1196,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>300</v>
@@ -1218,7 +1226,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>150</v>
@@ -1249,7 +1257,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>800</v>
@@ -1278,7 +1286,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>200</v>
@@ -1309,7 +1317,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>1000</v>
@@ -1338,7 +1346,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
         <v>100</v>
@@ -1367,7 +1375,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
         <v>100</v>
@@ -1396,7 +1404,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
         <v>1500</v>
@@ -1427,7 +1435,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
         <v>230</v>
@@ -1456,7 +1464,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
         <v>500</v>
@@ -1486,7 +1494,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -1516,7 +1524,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1">
         <v>1200</v>
@@ -1546,7 +1554,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
         <v>300</v>
@@ -1576,7 +1584,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1">
         <v>700</v>
@@ -1606,7 +1614,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1">
         <v>20</v>
@@ -1636,7 +1644,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1">
         <v>900</v>
@@ -1667,7 +1675,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1">
         <v>500</v>
@@ -1697,7 +1705,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1">
         <v>1400</v>
@@ -1727,7 +1735,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1">
         <v>100</v>
@@ -1757,7 +1765,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1">
         <v>60</v>
@@ -1787,7 +1795,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1">
         <v>500</v>
@@ -1817,7 +1825,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
         <v>700</v>
@@ -1847,7 +1855,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -1877,7 +1885,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1">
         <v>300</v>
@@ -1907,7 +1915,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1">
         <v>50</v>
@@ -1937,7 +1945,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1">
         <v>20</v>
@@ -1967,7 +1975,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1">
         <v>900</v>
@@ -1997,7 +2005,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1">
         <v>140</v>
@@ -2027,7 +2035,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1">
         <v>60</v>
@@ -2057,7 +2065,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1">
         <v>10</v>
@@ -2087,7 +2095,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1">
         <v>700</v>
@@ -2117,7 +2125,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1">
         <v>500</v>
@@ -2238,6 +2246,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C4ABA94203F5748B109EBB7A2B66A24" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b14cb3232c46c11352faa6e192ede145">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="606bd0ba-55e6-434f-bf07-749f78accee2" xmlns:ns4="21f765a5-c597-45a3-897b-84f427d866ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84b2d4089f6effa903dbee879072b2e8" ns3:_="" ns4:_="">
     <xsd:import namespace="606bd0ba-55e6-434f-bf07-749f78accee2"/>
@@ -2466,15 +2483,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2482,6 +2490,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3A1D81-B79C-470C-B259-EF659D59E72C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0865417-1B09-4DF2-BA06-A69EF24AD5DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2500,14 +2516,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3A1D81-B79C-470C-B259-EF659D59E72C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2163975D-6C90-4D2B-867A-E7435F56DE12}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
First start of renaming out -> outstanding
</commit_message>
<xml_diff>
--- a/tno/quantum/problems/portfolio_optimization/datasets/rabodata.xlsx
+++ b/tno/quantum/problems/portfolio_optimization/datasets/rabodata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wezemanrs\Desktop\projects\Quantum-projects\QuantumToolbox\PROBLEMS\portfolio-optimization\tno\quantum\problems\portfolio_optimization\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F09AAD-0A9B-44EB-8BCE-AB295289DC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A1739E-A106-474F-BD5E-9D016B5FA52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="360" windowWidth="20955" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="43200" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,15 +191,6 @@
     <t>Packaging &amp; Logistics COUNTRY 4</t>
   </si>
   <si>
-    <t>out_now</t>
-  </si>
-  <si>
-    <t>out_future_min</t>
-  </si>
-  <si>
-    <t>out_future_max</t>
-  </si>
-  <si>
     <t>emis_intens_now</t>
   </si>
   <si>
@@ -213,6 +204,15 @@
   </si>
   <si>
     <t>asset</t>
+  </si>
+  <si>
+    <t>outstanding_now</t>
+  </si>
+  <si>
+    <t>outstanding_future_min</t>
+  </si>
+  <si>
+    <t>outstanding_future_max</t>
   </si>
 </sst>
 </file>
@@ -548,15 +548,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
@@ -566,28 +566,28 @@
   <sheetData>
     <row r="1" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>